<commit_message>
Added attention result with 100 epochs
</commit_message>
<xml_diff>
--- a/reports/results_overview.xlsx
+++ b/reports/results_overview.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t xml:space="preserve">20210429-131938</t>
+  </si>
+  <si>
+    <t xml:space="preserve">InceptV3_LSTM_Attention_CustEmbedding</t>
   </si>
 </sst>
 </file>
@@ -152,7 +155,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -167,6 +170,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -186,15 +193,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.76953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="46.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="51.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.42"/>
@@ -271,6 +278,29 @@
       </c>
       <c r="H3" s="1" t="n">
         <v>0.5794</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>0.3015</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>0.3015</v>
+      </c>
+      <c r="G4" s="4" t="n">
+        <v>0.5192</v>
+      </c>
+      <c r="H4" s="4" t="n">
+        <v>0.5299</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final results run 20210429-131938
</commit_message>
<xml_diff>
--- a/reports/results_overview.xlsx
+++ b/reports/results_overview.xlsx
@@ -78,8 +78,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -155,7 +156,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -172,8 +173,12 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -193,13 +198,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="51.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.28"/>
@@ -234,7 +239,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>8</v>
       </c>
@@ -247,20 +252,20 @@
       <c r="D2" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="1" t="n">
+      <c r="E2" s="4" t="n">
         <v>0.357821684511512</v>
       </c>
-      <c r="F2" s="1" t="n">
+      <c r="F2" s="4" t="n">
         <v>0.400774315860991</v>
       </c>
-      <c r="G2" s="1" t="n">
+      <c r="G2" s="4" t="n">
         <v>0.514903454558174</v>
       </c>
-      <c r="H2" s="1" t="n">
+      <c r="H2" s="4" t="n">
         <v>0.590104876462518</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>12</v>
       </c>
@@ -273,11 +278,17 @@
       <c r="D3" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="1" t="n">
-        <v>0.5093</v>
-      </c>
-      <c r="H3" s="1" t="n">
-        <v>0.5794</v>
+      <c r="E3" s="4" t="n">
+        <v>0.364595036529411</v>
+      </c>
+      <c r="F3" s="4" t="n">
+        <v>0.403574780101712</v>
+      </c>
+      <c r="G3" s="4" t="n">
+        <v>0.509321365387381</v>
+      </c>
+      <c r="H3" s="4" t="n">
+        <v>0.579446402898139</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -290,18 +301,102 @@
       <c r="C4" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="1" t="n">
+      <c r="E4" s="4" t="n">
         <v>0.3015</v>
       </c>
-      <c r="F4" s="1" t="n">
+      <c r="F4" s="4" t="n">
         <v>0.3015</v>
       </c>
-      <c r="G4" s="4" t="n">
+      <c r="G4" s="5" t="n">
         <v>0.5192</v>
       </c>
-      <c r="H4" s="4" t="n">
+      <c r="H4" s="5" t="n">
         <v>0.5299</v>
       </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
added Baseline + Glove Word vectors
</commit_message>
<xml_diff>
--- a/reports/results_overview.xlsx
+++ b/reports/results_overview.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
@@ -90,6 +90,18 @@
   </si>
   <si>
     <t xml:space="preserve">20210429-173000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baseline + Glove Word vectors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">InceptionV3 (2048 units)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LSTM (2048 units)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baseline + Glove Word vectors + 2x LSTM</t>
   </si>
 </sst>
 </file>
@@ -100,7 +112,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -131,6 +143,12 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -174,7 +192,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -197,6 +215,10 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -219,10 +241,10 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.82421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="51.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.28"/>
@@ -359,16 +381,50 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
+      <c r="A6" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="4" t="n">
+        <v>0.3592</v>
+      </c>
+      <c r="F6" s="4" t="n">
+        <v>0.3968</v>
+      </c>
+      <c r="G6" s="4" t="n">
+        <v>0.5893</v>
+      </c>
+      <c r="H6" s="4" t="n">
+        <v>0.6715</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
+      <c r="A7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="4" t="n">
+        <v>0.3515</v>
+      </c>
+      <c r="F7" s="4" t="n">
+        <v>0.2503</v>
+      </c>
+      <c r="G7" s="4" t="n">
+        <v>0.4028</v>
+      </c>
+      <c r="H7" s="4" t="n">
+        <v>0.2631</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E8" s="4"/>

</xml_diff>

<commit_message>
Backup of not finished changes
</commit_message>
<xml_diff>
--- a/reports/results_overview.xlsx
+++ b/reports/results_overview.xlsx
@@ -251,10 +251,10 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
+      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.90234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="51.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.28"/>
@@ -482,7 +482,7 @@
         <v>0.4401</v>
       </c>
       <c r="G9" s="1" t="n">
-        <v>0.4934</v>
+        <v>0.4023</v>
       </c>
       <c r="H9" s="4" t="n">
         <v>0.4934</v>

</xml_diff>

<commit_message>
Corrected image preprocessing -> "_v2"
</commit_message>
<xml_diff>
--- a/reports/results_overview.xlsx
+++ b/reports/results_overview.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
@@ -114,6 +114,12 @@
   </si>
   <si>
     <t xml:space="preserve">20210430-201023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inception-ResNet-V2_GRU_NoAttention_CustEmbedding_V2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20210503-163216</t>
   </si>
 </sst>
 </file>
@@ -251,15 +257,15 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
+      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="51.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="5" style="1" width="15.57"/>
   </cols>
   <sheetData>
@@ -489,15 +495,33 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
+      <c r="A10" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="4" t="n">
+        <v>0.439543646042204</v>
+      </c>
+      <c r="F10" s="4" t="n">
+        <v>0.535184995762384</v>
+      </c>
+      <c r="G10" s="4" t="n">
+        <v>0.678756956522537</v>
+      </c>
+      <c r="H10" s="4" t="n">
+        <v>0.857577816799581</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E11" s="4"/>
       <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
       <c r="H11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
IndeptionV3 based models (version 2)
</commit_message>
<xml_diff>
--- a/reports/results_overview.xlsx
+++ b/reports/results_overview.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
@@ -116,10 +116,31 @@
     <t xml:space="preserve">20210430-201023</t>
   </si>
   <si>
+    <t xml:space="preserve">InceptV3_LSTM_NoAttention_CustEmbedding_V2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20210504-084723</t>
+  </si>
+  <si>
+    <t xml:space="preserve">InceptV3_GRU_NoAttention_CustEmbedding_V2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20210503-193008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.4287</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.5498</t>
+  </si>
+  <si>
     <t xml:space="preserve">Inception-ResNet-V2_GRU_NoAttention_CustEmbedding_V2</t>
   </si>
   <si>
     <t xml:space="preserve">20210503-163216</t>
+  </si>
+  <si>
+    <t xml:space="preserve">InceptV3_LSTM_Attention_CustEmbedding_V2</t>
   </si>
 </sst>
 </file>
@@ -136,7 +157,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -159,7 +179,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -204,7 +223,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -235,6 +254,10 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -254,22 +277,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:BL18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.94140625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="51.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="5" style="1" width="15.57"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="23.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -294,6 +317,62 @@
       <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+      <c r="AA1" s="2"/>
+      <c r="AB1" s="2"/>
+      <c r="AC1" s="2"/>
+      <c r="AD1" s="2"/>
+      <c r="AE1" s="2"/>
+      <c r="AF1" s="2"/>
+      <c r="AG1" s="2"/>
+      <c r="AH1" s="2"/>
+      <c r="AI1" s="2"/>
+      <c r="AJ1" s="2"/>
+      <c r="AK1" s="2"/>
+      <c r="AL1" s="2"/>
+      <c r="AM1" s="2"/>
+      <c r="AN1" s="2"/>
+      <c r="AO1" s="2"/>
+      <c r="AP1" s="2"/>
+      <c r="AQ1" s="2"/>
+      <c r="AR1" s="2"/>
+      <c r="AS1" s="2"/>
+      <c r="AT1" s="2"/>
+      <c r="AU1" s="2"/>
+      <c r="AV1" s="2"/>
+      <c r="AW1" s="2"/>
+      <c r="AX1" s="2"/>
+      <c r="AY1" s="2"/>
+      <c r="AZ1" s="2"/>
+      <c r="BA1" s="2"/>
+      <c r="BB1" s="2"/>
+      <c r="BC1" s="2"/>
+      <c r="BD1" s="2"/>
+      <c r="BE1" s="2"/>
+      <c r="BF1" s="2"/>
+      <c r="BG1" s="2"/>
+      <c r="BH1" s="2"/>
+      <c r="BI1" s="2"/>
+      <c r="BJ1" s="2"/>
+      <c r="BK1" s="2"/>
+      <c r="BL1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
@@ -494,49 +573,94 @@
         <v>0.4934</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B11" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="1" t="n">
+        <v>0.4277</v>
+      </c>
+      <c r="F11" s="1" t="n">
+        <v>0.5544</v>
+      </c>
+      <c r="G11" s="1" t="n">
+        <v>0.6599</v>
+      </c>
+      <c r="H11" s="4" t="n">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G12" s="4" t="n">
+        <v>0.671</v>
+      </c>
+      <c r="H12" s="4" t="n">
+        <v>0.8641</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C13" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="4" t="n">
+      <c r="D13" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="4" t="n">
         <v>0.439543646042204</v>
       </c>
-      <c r="F10" s="4" t="n">
+      <c r="F13" s="4" t="n">
         <v>0.535184995762384</v>
       </c>
-      <c r="G10" s="4" t="n">
+      <c r="G13" s="4" t="n">
         <v>0.678756956522537</v>
       </c>
-      <c r="H10" s="4" t="n">
+      <c r="H13" s="4" t="n">
         <v>0.857577816799581</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F11" s="4"/>
-      <c r="H11" s="4"/>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-    </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>10</v>
+      </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>

</xml_diff>